<commit_message>
some changes made in xml file
</commit_message>
<xml_diff>
--- a/testData/registeredAccounts.xlsx
+++ b/testData/registeredAccounts.xlsx
@@ -1311,7 +1311,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1380,7 +1380,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
@@ -1391,7 +1391,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
@@ -1402,7 +1402,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
@@ -1457,7 +1457,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
@@ -1495,6 +1495,10 @@
     <hyperlink ref="A4" r:id="rId1" display="dmpda@gmail.com" tooltip="mailto:dmpda@gmail.com"/>
     <hyperlink ref="A5" r:id="rId2" display="dmphu8da@gmail.com"/>
     <hyperlink ref="A6" r:id="rId3" display="hfdhdh@gmail.com"/>
+    <hyperlink ref="A7" r:id="rId4" display="ijfdl@gmail.com"/>
+    <hyperlink ref="A8" r:id="rId5" display="mnnul@gmail.com"/>
+    <hyperlink ref="A9" r:id="rId6" display="pybrr@gmail.com"/>
+    <hyperlink ref="A14" r:id="rId7" display="vxwxw@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>